<commit_message>
Auto stash before checking out "origin/main"
</commit_message>
<xml_diff>
--- a/suppxls/Scen_Localisation-Hi_NoPrice.xlsx
+++ b/suppxls/Scen_Localisation-Hi_NoPrice.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46425904-8EF3-4A44-B6A5-64E65C165DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99589280-E0D2-423F-B20C-2CAA11A70797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{232E471A-D1BC-46EA-822F-4A9C8F9BFC34}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{232E471A-D1BC-46EA-822F-4A9C8F9BFC34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -480,7 +480,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -839,9 +839,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -879,7 +879,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -985,7 +985,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1127,7 +1127,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1146,38 +1146,38 @@
   <dimension ref="B1:BL83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="BK35" sqref="BK35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" customWidth="1"/>
-    <col min="53" max="53" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" customWidth="1"/>
+    <col min="53" max="53" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:14">
       <c r="B1" s="32" t="s">
         <v>119</v>
       </c>
       <c r="C1" s="18"/>
     </row>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14">
       <c r="B2" s="19"/>
       <c r="C2" s="22"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14">
       <c r="B3" s="19" t="s">
         <v>136</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14">
       <c r="B4" s="19" t="s">
         <v>137</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14">
       <c r="B5" s="19"/>
       <c r="C5" s="22"/>
       <c r="G5" s="12">
@@ -1210,7 +1210,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14">
       <c r="B6" s="25"/>
       <c r="C6" s="26"/>
       <c r="E6" t="s">
@@ -1229,22 +1229,22 @@
       </c>
       <c r="I6" s="27">
         <f>SUMIFS(I$41:I$63,$C$41:$C$63,$E16,$F$41:$F$63,$C$3)</f>
-        <v>0.55000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="J6" s="27">
         <f t="shared" ref="J6:L6" si="0">SUMIFS(J$41:J$63,$C$41:$C$63,$E16,$F$41:$F$63,$C$3)</f>
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="K6" s="27">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
       <c r="L6" s="27">
         <f t="shared" si="0"/>
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14">
       <c r="E7" t="s">
         <v>11</v>
       </c>
@@ -1261,22 +1261,22 @@
       </c>
       <c r="I7" s="27">
         <f t="shared" ref="I7:L7" si="1">SUMIFS(I$41:I$63,$C$41:$C$63,$E17,$F$41:$F$63,$C$3)</f>
-        <v>0.55000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="J7" s="27">
         <f t="shared" si="1"/>
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="K7" s="27">
         <f t="shared" si="1"/>
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
       <c r="L7" s="27">
         <f t="shared" si="1"/>
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14">
       <c r="E8" t="s">
         <v>123</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>0.78098360655737697</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14">
       <c r="E9" t="s">
         <v>120</v>
       </c>
@@ -1340,12 +1340,12 @@
         <v>0.94827586206896552</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14">
       <c r="C12" s="10" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14">
       <c r="C14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1355,7 +1355,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14">
       <c r="C15" s="2" t="s">
         <v>1</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14">
       <c r="C16" s="3" t="s">
         <v>3</v>
       </c>
@@ -1410,25 +1410,25 @@
       </c>
       <c r="I16" s="5">
         <f>1-I6</f>
-        <v>0.44999999999999996</v>
+        <v>0.5</v>
       </c>
       <c r="J16" s="5">
         <f t="shared" ref="J16:L16" si="4">1-J6</f>
-        <v>0.30000000000000004</v>
+        <v>0.35</v>
       </c>
       <c r="K16" s="5">
         <f t="shared" si="4"/>
-        <v>0.25</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="L16" s="5">
         <f t="shared" si="4"/>
-        <v>0.15000000000000002</v>
+        <v>0.25</v>
       </c>
       <c r="N16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="3:64" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:64">
       <c r="C17" s="3" t="s">
         <v>4</v>
       </c>
@@ -1451,22 +1451,22 @@
       </c>
       <c r="I17" s="5">
         <f t="shared" ref="I17:K17" si="5">1-I7</f>
-        <v>0.44999999999999996</v>
+        <v>0.5</v>
       </c>
       <c r="J17" s="5">
         <f t="shared" si="5"/>
-        <v>0.30000000000000004</v>
+        <v>0.35</v>
       </c>
       <c r="K17" s="5">
         <f t="shared" si="5"/>
-        <v>0.25</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="L17" s="5">
         <f>1-L7</f>
-        <v>0.15000000000000002</v>
-      </c>
-    </row>
-    <row r="18" spans="3:64" x14ac:dyDescent="0.25">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="18" spans="3:64">
       <c r="C18" t="s">
         <v>121</v>
       </c>
@@ -1551,7 +1551,7 @@
       <c r="BK18" s="13"/>
       <c r="BL18" s="13"/>
     </row>
-    <row r="19" spans="3:64" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:64">
       <c r="C19" t="s">
         <v>122</v>
       </c>
@@ -1592,12 +1592,12 @@
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="3:64" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:64">
       <c r="AZ21" s="14" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="22" spans="3:64" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:64">
       <c r="T22" s="14" t="s">
         <v>106</v>
       </c>
@@ -1629,10 +1629,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="3:64" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:64">
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="3:64" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:64">
       <c r="U24" s="30" t="s">
         <v>135</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="3:64" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:64">
       <c r="T25" s="8" t="s">
         <v>22</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="26" spans="3:64" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:64">
       <c r="T26" s="9" t="s">
         <v>25</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="3:64" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:64">
       <c r="T27" s="9" t="s">
         <v>27</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="3:64" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:64">
       <c r="C28" s="10" t="s">
         <v>17</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="3:64" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:64">
       <c r="C29" s="16"/>
       <c r="D29" s="17" t="s">
         <v>12</v>
@@ -2200,7 +2200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="3:64" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:64">
       <c r="C30" s="19"/>
       <c r="D30" t="s">
         <v>13</v>
@@ -2328,7 +2328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="3:64" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:64">
       <c r="C31" s="19" t="s">
         <v>15</v>
       </c>
@@ -2467,7 +2467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="3:64" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:64">
       <c r="C32" s="19">
         <v>2019</v>
       </c>
@@ -2608,7 +2608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:62">
       <c r="C33" s="19">
         <v>2020</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:62">
       <c r="C34" s="25"/>
       <c r="D34" s="13"/>
       <c r="E34" s="13"/>
@@ -2871,7 +2871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:62">
       <c r="T35" s="9" t="s">
         <v>43</v>
       </c>
@@ -2988,7 +2988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:62">
       <c r="T36" s="9" t="s">
         <v>45</v>
       </c>
@@ -3105,7 +3105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:62">
       <c r="T37" s="9" t="s">
         <v>47</v>
       </c>
@@ -3207,7 +3207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:62" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:62" ht="23.4">
       <c r="B38" s="31" t="s">
         <v>114</v>
       </c>
@@ -3312,7 +3312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:62">
       <c r="T39" s="9" t="s">
         <v>51</v>
       </c>
@@ -3414,7 +3414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:62">
       <c r="C40" s="10" t="s">
         <v>115</v>
       </c>
@@ -3537,7 +3537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:62">
       <c r="C41" s="3" t="s">
         <v>8</v>
       </c>
@@ -3665,7 +3665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:62">
       <c r="C42" t="str">
         <f>C41</f>
         <v>cmach_e</v>
@@ -3794,7 +3794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:62">
       <c r="C43" t="str">
         <f>C42</f>
         <v>cmach_e</v>
@@ -3923,7 +3923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:62">
       <c r="C44" t="str">
         <f>C43</f>
         <v>cmach_e</v>
@@ -4074,7 +4074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:62">
       <c r="T45" t="s">
         <v>63</v>
       </c>
@@ -4191,7 +4191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:62">
       <c r="T46" t="s">
         <v>65</v>
       </c>
@@ -4308,7 +4308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:62">
       <c r="C47" s="10" t="s">
         <v>116</v>
       </c>
@@ -4428,7 +4428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:62">
       <c r="C48" s="3" t="s">
         <v>11</v>
       </c>
@@ -4571,7 +4571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:62">
       <c r="C49" t="str">
         <f>C48</f>
         <v>cemch_e</v>
@@ -4715,7 +4715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:62">
       <c r="C50" t="str">
         <f>C49</f>
         <v>cemch_e</v>
@@ -4786,7 +4786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:62">
       <c r="C51" t="str">
         <f>C50</f>
         <v>cemch_e</v>
@@ -4858,7 +4858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:62">
       <c r="T52" s="9" t="s">
         <v>77</v>
       </c>
@@ -4896,7 +4896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:62">
       <c r="C53" s="10" t="s">
         <v>117</v>
       </c>
@@ -4937,7 +4937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:62">
       <c r="C54" t="s">
         <v>128</v>
       </c>
@@ -5009,7 +5009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:62">
       <c r="C55" t="s">
         <v>128</v>
       </c>
@@ -5077,7 +5077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:62">
       <c r="C56" t="s">
         <v>128</v>
       </c>
@@ -5144,7 +5144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:62">
       <c r="C57" t="s">
         <v>128</v>
       </c>
@@ -5209,7 +5209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:62">
       <c r="T58" s="9" t="s">
         <v>89</v>
       </c>
@@ -5241,7 +5241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:62">
       <c r="C59" s="10" t="s">
         <v>118</v>
       </c>
@@ -5276,7 +5276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:62">
       <c r="C60" s="3" t="s">
         <v>123</v>
       </c>
@@ -5342,7 +5342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:62">
       <c r="C61" t="str">
         <f>C60</f>
         <v>cmetp</v>
@@ -5405,7 +5405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:62">
       <c r="C62" t="str">
         <f>C61</f>
         <v>cmetp</v>
@@ -5468,7 +5468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:62">
       <c r="C63" t="str">
         <f>C62</f>
         <v>cmetp</v>
@@ -5534,7 +5534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:62">
       <c r="T64" s="9" t="s">
         <v>101</v>
       </c>
@@ -5566,7 +5566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="2:62" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:62" ht="23.4">
       <c r="B65" s="31" t="s">
         <v>134</v>
       </c>
@@ -5601,7 +5601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:62">
       <c r="F66" t="s">
         <v>111</v>
       </c>
@@ -5626,7 +5626,7 @@
       <c r="V66" s="9"/>
       <c r="W66" s="9"/>
     </row>
-    <row r="67" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:62">
       <c r="F67" t="s">
         <v>112</v>
       </c>
@@ -5649,7 +5649,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="68" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:62">
       <c r="F68" t="s">
         <v>113</v>
       </c>
@@ -5672,7 +5672,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="69" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:62">
       <c r="F69" t="s">
         <v>138</v>
       </c>
@@ -5695,7 +5695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:62">
       <c r="G79" t="s">
         <v>129</v>
       </c>
@@ -5712,7 +5712,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="80" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:62">
       <c r="F80" t="s">
         <v>128</v>
       </c>
@@ -5730,7 +5730,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="81" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="6:10">
       <c r="G81" s="4">
         <f>G80/I80</f>
         <v>6.1576354679802957E-2</v>
@@ -5740,7 +5740,7 @@
         <v>9.852216748768473E-3</v>
       </c>
     </row>
-    <row r="82" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="6:10">
       <c r="F82" t="s">
         <v>133</v>
       </c>
@@ -5758,7 +5758,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="83" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="6:10">
       <c r="G83" s="29">
         <f>G82/I82</f>
         <v>0.23934426229508196</v>

</xml_diff>